<commit_message>
fix: Refine `tipologia_istituto` values in institutional data and add a script to convert JSON to Excel.
</commit_message>
<xml_diff>
--- a/data/pna-istituzioni-afam.xlsx
+++ b/data/pna-istituzioni-afam.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J201"/>
+  <dimension ref="A1:J200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,11 +526,15 @@
           <t>www.acmemilano.it</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>45.479195</v>
-      </c>
-      <c r="J2" t="n">
-        <v>9.1727151</v>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>45.4791950</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>9.1727151</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -541,7 +545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -570,11 +574,15 @@
           <t>www.abadir.net</t>
         </is>
       </c>
-      <c r="I3" t="n">
-        <v>37.5023612</v>
-      </c>
-      <c r="J3" t="n">
-        <v>15.0873718</v>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>37.5023612</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>15.0873718</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -585,7 +593,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -618,11 +626,15 @@
           <t>www.accademiadellusso.com</t>
         </is>
       </c>
-      <c r="I4" t="n">
-        <v>45.4641943</v>
-      </c>
-      <c r="J4" t="n">
-        <v>9.1896346</v>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>45.4641943</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>9.1896346</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -633,7 +645,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -666,11 +678,15 @@
           <t>www.accademiamoda.it</t>
         </is>
       </c>
-      <c r="I5" t="n">
-        <v>45.4870381</v>
-      </c>
-      <c r="J5" t="n">
-        <v>9.199961800000001</v>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>45.4870381</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>9.1999618</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -681,7 +697,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -714,11 +730,15 @@
           <t>www.accademiamoda.it</t>
         </is>
       </c>
-      <c r="I6" t="n">
-        <v>40.8516689</v>
-      </c>
-      <c r="J6" t="n">
-        <v>14.2710407</v>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>40.8516689</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>14.2710407</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -729,7 +749,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -758,11 +778,15 @@
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="n">
-        <v>40.8485748</v>
-      </c>
-      <c r="J7" t="n">
-        <v>14.2754121</v>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>40.8485748</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>14.2754121</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -806,11 +830,15 @@
           <t>www.accademiadellearti.it/</t>
         </is>
       </c>
-      <c r="I8" t="n">
-        <v>41.8995826</v>
-      </c>
-      <c r="J8" t="n">
-        <v>12.4615198</v>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>41.8995826</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>12.4615198</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -854,11 +882,15 @@
           <t>www.accademiagalli.it</t>
         </is>
       </c>
-      <c r="I9" t="n">
-        <v>45.8114028</v>
-      </c>
-      <c r="J9" t="n">
-        <v>9.082948200000001</v>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>45.8114028</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>9.0829482</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -902,11 +934,15 @@
           <t>www.accademiatiepolo.it</t>
         </is>
       </c>
-      <c r="I10" t="n">
-        <v>46.0612126</v>
-      </c>
-      <c r="J10" t="n">
-        <v>13.2429135</v>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>46.0612126</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>13.2429135</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -950,11 +986,15 @@
           <t>www.abav.it/</t>
         </is>
       </c>
-      <c r="I11" t="n">
-        <v>42.4168437</v>
-      </c>
-      <c r="J11" t="n">
-        <v>12.1051483</v>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>42.4168437</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>12.1051483</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -998,11 +1038,15 @@
           <t>www.accademiasantagiulia.it</t>
         </is>
       </c>
-      <c r="I12" t="n">
-        <v>45.5400283</v>
-      </c>
-      <c r="J12" t="n">
-        <v>10.2200316</v>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>45.5400283</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>10.2200316</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -1046,11 +1090,15 @@
           <t>www.trentinoartacademy.it</t>
         </is>
       </c>
-      <c r="I13" t="n">
-        <v>46.0903634</v>
-      </c>
-      <c r="J13" t="n">
-        <v>11.1169593</v>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>46.0903634</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>11.1169593</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -1094,11 +1142,15 @@
           <t>www.abaq.it</t>
         </is>
       </c>
-      <c r="I14" t="n">
-        <v>42.3657587</v>
-      </c>
-      <c r="J14" t="n">
-        <v>13.3699383</v>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>42.3657587</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>13.3699383</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -1142,11 +1194,15 @@
           <t>www.accademiabelleartiba.it/</t>
         </is>
       </c>
-      <c r="I15" t="n">
-        <v>41.1111309</v>
-      </c>
-      <c r="J15" t="n">
-        <v>16.8763707</v>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>41.1111309</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>16.8763707</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -1190,11 +1246,15 @@
           <t>www.ababo.it</t>
         </is>
       </c>
-      <c r="I16" t="n">
-        <v>44.49778</v>
-      </c>
-      <c r="J16" t="n">
-        <v>11.3530204</v>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>44.4977800</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>11.3530204</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -1238,11 +1298,15 @@
           <t>www.abacatania.it</t>
         </is>
       </c>
-      <c r="I17" t="n">
-        <v>37.5300133</v>
-      </c>
-      <c r="J17" t="n">
-        <v>15.0788389</v>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>37.5300133</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>15.0788389</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -1286,11 +1350,15 @@
           <t>www.conservatoriocuneo.it</t>
         </is>
       </c>
-      <c r="I18" t="n">
-        <v>44.3931767</v>
-      </c>
-      <c r="J18" t="n">
-        <v>7.551703</v>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>44.3931767</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>7.5517030</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -1334,11 +1402,15 @@
           <t>www.accademia.firenze.it</t>
         </is>
       </c>
-      <c r="I19" t="n">
-        <v>43.7762373</v>
-      </c>
-      <c r="J19" t="n">
-        <v>11.2581792</v>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>43.7762373</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>11.2581792</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -1382,11 +1454,15 @@
           <t>www.abafg.it</t>
         </is>
       </c>
-      <c r="I20" t="n">
-        <v>41.784193</v>
-      </c>
-      <c r="J20" t="n">
-        <v>15.4422824</v>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>41.7841930</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>15.4422824</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -1430,11 +1506,15 @@
           <t>www.abana.it</t>
         </is>
       </c>
-      <c r="I21" t="n">
-        <v>40.8736035</v>
-      </c>
-      <c r="J21" t="n">
-        <v>14.4688388</v>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>40.8736035</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>14.4688388</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -1478,11 +1558,15 @@
           <t>www.abarc.it</t>
         </is>
       </c>
-      <c r="I22" t="n">
-        <v>38.2618287</v>
-      </c>
-      <c r="J22" t="n">
-        <v>15.8558228</v>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>38.2618287</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>15.8558228</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -1526,11 +1610,15 @@
           <t>www.abaroma.it/</t>
         </is>
       </c>
-      <c r="I23" t="n">
-        <v>41.9985375</v>
-      </c>
-      <c r="J23" t="n">
-        <v>12.0984639</v>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>41.9985375</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>12.0984639</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -1574,11 +1662,15 @@
           <t>www.accademiabelleartisanremo.it</t>
         </is>
       </c>
-      <c r="I24" t="n">
-        <v>43.8248461</v>
-      </c>
-      <c r="J24" t="n">
-        <v>7.7812209</v>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>43.8248461</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>7.7812209</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -1622,11 +1714,15 @@
           <t>www.accademiasironi.it</t>
         </is>
       </c>
-      <c r="I25" t="n">
-        <v>40.7176102</v>
-      </c>
-      <c r="J25" t="n">
-        <v>8.5702339</v>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>40.7176102</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>8.5702339</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -1670,11 +1766,15 @@
           <t>www.accademiavenezia.it/</t>
         </is>
       </c>
-      <c r="I26" t="n">
-        <v>45.4331323</v>
-      </c>
-      <c r="J26" t="n">
-        <v>12.3190338</v>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>45.4331323</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>12.3190338</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -1714,11 +1814,15 @@
         </is>
       </c>
       <c r="H27" t="inlineStr"/>
-      <c r="I27" t="n">
-        <v>43.60763</v>
-      </c>
-      <c r="J27" t="n">
-        <v>13.513087</v>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>43.6076300</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>13.5130870</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -1762,11 +1866,15 @@
           <t>www.accademiabelleartisanremo.it/it/</t>
         </is>
       </c>
-      <c r="I28" t="n">
-        <v>45.4998314</v>
-      </c>
-      <c r="J28" t="n">
-        <v>9.2192945</v>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>45.4998314</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>9.2192945</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -1810,11 +1918,15 @@
           <t>www.madeprogram.it/</t>
         </is>
       </c>
-      <c r="I29" t="n">
-        <v>37.0646531</v>
-      </c>
-      <c r="J29" t="n">
-        <v>15.2879551</v>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>37.0646531</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>15.2879551</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -1858,11 +1970,15 @@
           <t>www.accademiabellearticuneo.it</t>
         </is>
       </c>
-      <c r="I30" t="n">
-        <v>44.3895006</v>
-      </c>
-      <c r="J30" t="n">
-        <v>7.5477909</v>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>44.3895006</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>7.5477909</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -1906,11 +2022,15 @@
           <t>www.naba.it</t>
         </is>
       </c>
-      <c r="I31" t="n">
-        <v>41.867863</v>
-      </c>
-      <c r="J31" t="n">
-        <v>12.4791773</v>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>41.8678630</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>12.4791773</t>
+        </is>
       </c>
     </row>
     <row r="32">
@@ -1954,11 +2074,15 @@
           <t>www.consba.it/</t>
         </is>
       </c>
-      <c r="I32" t="n">
-        <v>41.1157586</v>
-      </c>
-      <c r="J32" t="n">
-        <v>16.8568829</v>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>41.1157586</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>16.8568829</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -2002,11 +2126,15 @@
           <t>www.consbo.it</t>
         </is>
       </c>
-      <c r="I33" t="n">
-        <v>44.4952952</v>
-      </c>
-      <c r="J33" t="n">
-        <v>11.3490593</v>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>44.4952952</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>11.3490593</t>
+        </is>
       </c>
     </row>
     <row r="34">
@@ -2050,11 +2178,15 @@
           <t>www.accademiacarrara.it</t>
         </is>
       </c>
-      <c r="I34" t="n">
-        <v>44.0784425</v>
-      </c>
-      <c r="J34" t="n">
-        <v>10.099423</v>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>44.0784425</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>10.0994230</t>
+        </is>
       </c>
     </row>
     <row r="35">
@@ -2098,11 +2230,15 @@
           <t>www.abacatanzaro.it</t>
         </is>
       </c>
-      <c r="I35" t="n">
-        <v>38.9173324</v>
-      </c>
-      <c r="J35" t="n">
-        <v>16.5688438</v>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>38.9173324</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>16.5688438</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -2146,11 +2282,15 @@
           <t>www.consfi.it/</t>
         </is>
       </c>
-      <c r="I36" t="n">
-        <v>43.7763996</v>
-      </c>
-      <c r="J36" t="n">
-        <v>11.2583489</v>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>43.7763996</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>11.2583489</t>
+        </is>
       </c>
     </row>
     <row r="37">
@@ -2194,11 +2334,15 @@
           <t>www.conservatoriofoggia.it</t>
         </is>
       </c>
-      <c r="I37" t="n">
-        <v>41.5028106</v>
-      </c>
-      <c r="J37" t="n">
-        <v>15.4528939</v>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>41.5028106</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>15.4528939</t>
+        </is>
       </c>
     </row>
     <row r="38">
@@ -2242,11 +2386,15 @@
           <t>www.accademiabellearti.fr.it</t>
         </is>
       </c>
-      <c r="I38" t="n">
-        <v>41.5775271</v>
-      </c>
-      <c r="J38" t="n">
-        <v>13.6059872</v>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>41.5775271</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>13.6059872</t>
+        </is>
       </c>
     </row>
     <row r="39">
@@ -2290,11 +2438,15 @@
           <t>www.accademialigustica.it/</t>
         </is>
       </c>
-      <c r="I39" t="n">
-        <v>44.4076284</v>
-      </c>
-      <c r="J39" t="n">
-        <v>8.9348449</v>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>44.4076284</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>8.9348449</t>
+        </is>
       </c>
     </row>
     <row r="40">
@@ -2338,11 +2490,15 @@
           <t>WWW.CONSAQ.IT</t>
         </is>
       </c>
-      <c r="I40" t="n">
-        <v>42.3505221</v>
-      </c>
-      <c r="J40" t="n">
-        <v>13.3964753</v>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>42.3505221</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>13.3964753</t>
+        </is>
       </c>
     </row>
     <row r="41">
@@ -2386,11 +2542,15 @@
           <t>www.accademialecce.edu.it/</t>
         </is>
       </c>
-      <c r="I41" t="n">
-        <v>40.3512613</v>
-      </c>
-      <c r="J41" t="n">
-        <v>18.1646249</v>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>40.3512613</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>18.1646249</t>
+        </is>
       </c>
     </row>
     <row r="42">
@@ -2434,11 +2594,15 @@
           <t>www.abamc.it</t>
         </is>
       </c>
-      <c r="I42" t="n">
-        <v>43.3010295</v>
-      </c>
-      <c r="J42" t="n">
-        <v>13.4508955</v>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>43.3010295</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>13.4508955</t>
+        </is>
       </c>
     </row>
     <row r="43">
@@ -2482,11 +2646,15 @@
           <t>www.accademiadibrera.milano.it</t>
         </is>
       </c>
-      <c r="I43" t="n">
-        <v>45.4722421</v>
-      </c>
-      <c r="J43" t="n">
-        <v>9.188407099999999</v>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>45.4722421</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>9.1884071</t>
+        </is>
       </c>
     </row>
     <row r="44">
@@ -2530,11 +2698,15 @@
           <t>www.sanpietroamajella.it</t>
         </is>
       </c>
-      <c r="I44" t="n">
-        <v>40.8358846</v>
-      </c>
-      <c r="J44" t="n">
-        <v>14.2487679</v>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>40.8358846</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>14.2487679</t>
+        </is>
       </c>
     </row>
     <row r="45">
@@ -2578,11 +2750,15 @@
           <t>www.accademiadipalermo.it</t>
         </is>
       </c>
-      <c r="I45" t="n">
-        <v>38.1163595</v>
-      </c>
-      <c r="J45" t="n">
-        <v>13.3522738</v>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>38.1163595</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>13.3522738</t>
+        </is>
       </c>
     </row>
     <row r="46">
@@ -2626,11 +2802,15 @@
           <t>www.abaperugia.org</t>
         </is>
       </c>
-      <c r="I46" t="n">
-        <v>43.1130349</v>
-      </c>
-      <c r="J46" t="n">
-        <v>12.38441</v>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>43.1130349</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>12.3844100</t>
+        </is>
       </c>
     </row>
     <row r="47">
@@ -2674,11 +2854,15 @@
           <t>www.abaravenna.it</t>
         </is>
       </c>
-      <c r="I47" t="n">
-        <v>44.4262085</v>
-      </c>
-      <c r="J47" t="n">
-        <v>12.2137298</v>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>44.4262085</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>12.2137298</t>
+        </is>
       </c>
     </row>
     <row r="48">
@@ -2718,11 +2902,15 @@
         </is>
       </c>
       <c r="H48" t="inlineStr"/>
-      <c r="I48" t="n">
-        <v>41.9074985</v>
-      </c>
-      <c r="J48" t="n">
-        <v>12.4788258</v>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>41.9074985</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>12.4788258</t>
+        </is>
       </c>
     </row>
     <row r="49">
@@ -2766,11 +2954,15 @@
           <t>www.albertina.academy</t>
         </is>
       </c>
-      <c r="I49" t="n">
-        <v>45.0675807</v>
-      </c>
-      <c r="J49" t="n">
-        <v>7.6897297</v>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>45.0675807</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>7.6897297</t>
+        </is>
       </c>
     </row>
     <row r="50">
@@ -2814,11 +3006,15 @@
           <t>www.accademiadiurbino.it</t>
         </is>
       </c>
-      <c r="I50" t="n">
-        <v>43.7275794</v>
-      </c>
-      <c r="J50" t="n">
-        <v>12.6341966</v>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>43.7275794</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>12.6341966</t>
+        </is>
       </c>
     </row>
     <row r="51">
@@ -2862,11 +3058,15 @@
           <t>www.accademiavenezia.it</t>
         </is>
       </c>
-      <c r="I51" t="n">
-        <v>45.4371908</v>
-      </c>
-      <c r="J51" t="n">
-        <v>12.3345898</v>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>45.4371908</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>12.3345898</t>
+        </is>
       </c>
     </row>
     <row r="52">
@@ -2910,11 +3110,15 @@
           <t>www.accademiabelleartiverona.it/it/</t>
         </is>
       </c>
-      <c r="I52" t="n">
-        <v>45.4989147</v>
-      </c>
-      <c r="J52" t="n">
-        <v>10.9390044</v>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>45.4989147</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>10.9390044</t>
+        </is>
       </c>
     </row>
     <row r="53">
@@ -2925,7 +3129,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2958,11 +3162,15 @@
           <t>www.accademiacostumeemoda.it</t>
         </is>
       </c>
-      <c r="I53" t="n">
-        <v>41.9011272</v>
-      </c>
-      <c r="J53" t="n">
-        <v>12.468626</v>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>41.9011272</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>12.4686260</t>
+        </is>
       </c>
     </row>
     <row r="54">
@@ -2973,7 +3181,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -3006,11 +3214,15 @@
           <t>www.accademiacostumeemoda.it</t>
         </is>
       </c>
-      <c r="I54" t="n">
-        <v>45.4576097</v>
-      </c>
-      <c r="J54" t="n">
-        <v>9.209433499999999</v>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>45.4576097</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>9.2094335</t>
+        </is>
       </c>
     </row>
     <row r="55">
@@ -3050,11 +3262,15 @@
         </is>
       </c>
       <c r="H55" t="inlineStr"/>
-      <c r="I55" t="n">
-        <v>37.5590533</v>
-      </c>
-      <c r="J55" t="n">
-        <v>15.0829428</v>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>37.5590533</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>15.0829428</t>
+        </is>
       </c>
     </row>
     <row r="56">
@@ -3098,11 +3314,15 @@
           <t>www.scuoladiteatro.it</t>
         </is>
       </c>
-      <c r="I56" t="n">
-        <v>41.8716855</v>
-      </c>
-      <c r="J56" t="n">
-        <v>12.516649</v>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>41.8716855</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>12.5166490</t>
+        </is>
       </c>
     </row>
     <row r="57">
@@ -3113,7 +3333,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -3146,11 +3366,15 @@
           <t>www.accademiaitaliana.com</t>
         </is>
       </c>
-      <c r="I57" t="n">
-        <v>43.7700182</v>
-      </c>
-      <c r="J57" t="n">
-        <v>11.2556355</v>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>43.7700182</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>11.2556355</t>
+        </is>
       </c>
     </row>
     <row r="58">
@@ -3161,7 +3385,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -3194,11 +3418,15 @@
           <t>www.accademiaitaliana.com</t>
         </is>
       </c>
-      <c r="I58" t="n">
-        <v>41.8931171</v>
-      </c>
-      <c r="J58" t="n">
-        <v>12.5183989</v>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>41.8931171</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>12.5183989</t>
+        </is>
       </c>
     </row>
     <row r="59">
@@ -3209,7 +3437,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -3238,11 +3466,15 @@
         </is>
       </c>
       <c r="H59" t="inlineStr"/>
-      <c r="I59" t="n">
-        <v>43.765542</v>
-      </c>
-      <c r="J59" t="n">
-        <v>11.2498414</v>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>43.7655420</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>11.2498414</t>
+        </is>
       </c>
     </row>
     <row r="60">
@@ -3286,11 +3518,15 @@
           <t>www.accademiasilviodamico.it</t>
         </is>
       </c>
-      <c r="I60" t="n">
-        <v>41.9200518</v>
-      </c>
-      <c r="J60" t="n">
-        <v>12.4937857</v>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>41.9200518</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>12.4937857</t>
+        </is>
       </c>
     </row>
     <row r="61">
@@ -3334,11 +3570,15 @@
           <t>www.accademianazionaledanza.it</t>
         </is>
       </c>
-      <c r="I61" t="n">
-        <v>41.8839516</v>
-      </c>
-      <c r="J61" t="n">
-        <v>12.4831017</v>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>41.8839516</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>12.4831017</t>
+        </is>
       </c>
     </row>
     <row r="62">
@@ -3382,11 +3622,15 @@
           <t>www.sienajazz.it/</t>
         </is>
       </c>
-      <c r="I62" t="n">
-        <v>43.3189467</v>
-      </c>
-      <c r="J62" t="n">
-        <v>11.3316569</v>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>43.3189467</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>11.3316569</t>
+        </is>
       </c>
     </row>
     <row r="63">
@@ -3430,11 +3674,15 @@
           <t>www.accademialascala.it</t>
         </is>
       </c>
-      <c r="I63" t="n">
-        <v>45.4617877</v>
-      </c>
-      <c r="J63" t="n">
-        <v>9.182393299999999</v>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>45.4617877</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>9.1823933</t>
+        </is>
       </c>
     </row>
     <row r="64">
@@ -3478,11 +3726,15 @@
           <t>https://cinema.fondazionemilano.eu/</t>
         </is>
       </c>
-      <c r="I64" t="n">
-        <v>45.5135671</v>
-      </c>
-      <c r="J64" t="n">
-        <v>9.2040168</v>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>45.5135671</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>9.2040168</t>
+        </is>
       </c>
     </row>
     <row r="65">
@@ -3493,7 +3745,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Istituti Musicali</t>
+          <t>Altro</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -3526,11 +3778,15 @@
           <t>https://musica.fondazionemilano.eu/</t>
         </is>
       </c>
-      <c r="I65" t="n">
-        <v>45.491115</v>
-      </c>
-      <c r="J65" t="n">
-        <v>9.1683073</v>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>45.4911150</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>9.1683073</t>
+        </is>
       </c>
     </row>
     <row r="66">
@@ -3541,7 +3797,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Istituti di Teatro e Coreutica</t>
+          <t>Altro</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -3574,11 +3830,15 @@
           <t>https://teatro.fondazionemilano.eu/</t>
         </is>
       </c>
-      <c r="I66" t="n">
-        <v>45.4500411</v>
-      </c>
-      <c r="J66" t="n">
-        <v>9.192546800000001</v>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>45.4500411</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>9.1925468</t>
+        </is>
       </c>
     </row>
     <row r="67">
@@ -3622,11 +3882,15 @@
           <t>https://lingue.fondazionemilano.eu/</t>
         </is>
       </c>
-      <c r="I67" t="n">
-        <v>45.4558459</v>
-      </c>
-      <c r="J67" t="n">
-        <v>9.1719563</v>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>45.4558459</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>9.1719563</t>
+        </is>
       </c>
     </row>
     <row r="68">
@@ -3670,11 +3934,15 @@
           <t>www.conservatorioadria.it</t>
         </is>
       </c>
-      <c r="I68" t="n">
-        <v>45.0591181</v>
-      </c>
-      <c r="J68" t="n">
-        <v>12.0547219</v>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>45.0591181</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>12.0547219</t>
+        </is>
       </c>
     </row>
     <row r="69">
@@ -3718,11 +3986,15 @@
           <t>www.cons.bz.it</t>
         </is>
       </c>
-      <c r="I69" t="n">
-        <v>46.4976732</v>
-      </c>
-      <c r="J69" t="n">
-        <v>11.3515688</v>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>46.4976732</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>11.3515688</t>
+        </is>
       </c>
     </row>
     <row r="70">
@@ -3766,11 +4038,15 @@
           <t>www.consbs.it</t>
         </is>
       </c>
-      <c r="I70" t="n">
-        <v>45.5358028</v>
-      </c>
-      <c r="J70" t="n">
-        <v>10.2255838</v>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>45.5358028</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>10.2255838</t>
+        </is>
       </c>
     </row>
     <row r="71">
@@ -3814,11 +4090,15 @@
           <t>www.conservatoriocomo.it</t>
         </is>
       </c>
-      <c r="I71" t="n">
-        <v>45.7940756</v>
-      </c>
-      <c r="J71" t="n">
-        <v>9.1176447</v>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>45.7940756</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>9.1176447</t>
+        </is>
       </c>
     </row>
     <row r="72">
@@ -3862,11 +4142,15 @@
           <t>www.conservatorio.net</t>
         </is>
       </c>
-      <c r="I72" t="n">
-        <v>43.1617794</v>
-      </c>
-      <c r="J72" t="n">
-        <v>13.7173919</v>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>43.1617794</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>13.7173919</t>
+        </is>
       </c>
     </row>
     <row r="73">
@@ -3910,11 +4194,15 @@
           <t>www.conservatoriofoggia.it</t>
         </is>
       </c>
-      <c r="I73" t="n">
-        <v>41.9289048</v>
-      </c>
-      <c r="J73" t="n">
-        <v>15.8802919</v>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>41.9289048</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>15.8802919</t>
+        </is>
       </c>
     </row>
     <row r="74">
@@ -3958,11 +4246,15 @@
           <t>www.conservatorio-frosinone.it</t>
         </is>
       </c>
-      <c r="I74" t="n">
-        <v>41.6285468</v>
-      </c>
-      <c r="J74" t="n">
-        <v>13.5758498</v>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>41.6285468</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>13.5758498</t>
+        </is>
       </c>
     </row>
     <row r="75">
@@ -4006,11 +4298,15 @@
           <t>www.conspaganini.it/</t>
         </is>
       </c>
-      <c r="I75" t="n">
-        <v>44.4008022</v>
-      </c>
-      <c r="J75" t="n">
-        <v>8.958120600000001</v>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>44.4008022</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>8.9581206</t>
+        </is>
       </c>
     </row>
     <row r="76">
@@ -4054,11 +4350,15 @@
           <t>www.conservatoriolecce.it</t>
         </is>
       </c>
-      <c r="I76" t="n">
-        <v>40.1522173</v>
-      </c>
-      <c r="J76" t="n">
-        <v>18.2260628</v>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>40.1522173</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>18.2260628</t>
+        </is>
       </c>
     </row>
     <row r="77">
@@ -4102,11 +4402,15 @@
           <t>www.conservatoriolecce.it</t>
         </is>
       </c>
-      <c r="I77" t="n">
-        <v>40.6460444</v>
-      </c>
-      <c r="J77" t="n">
-        <v>17.5170566</v>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>40.6460444</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>17.5170566</t>
+        </is>
       </c>
     </row>
     <row r="78">
@@ -4150,11 +4454,15 @@
           <t>www.boccherini.it</t>
         </is>
       </c>
-      <c r="I78" t="n">
-        <v>43.8428399</v>
-      </c>
-      <c r="J78" t="n">
-        <v>10.5062918</v>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>43.8428399</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>10.5062918</t>
+        </is>
       </c>
     </row>
     <row r="79">
@@ -4198,11 +4506,15 @@
           <t>www.consmi.it</t>
         </is>
       </c>
-      <c r="I79" t="n">
-        <v>45.4650024</v>
-      </c>
-      <c r="J79" t="n">
-        <v>9.203199400000001</v>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>45.4650024</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>9.2031994</t>
+        </is>
       </c>
     </row>
     <row r="80">
@@ -4246,11 +4558,15 @@
           <t>www.vecchitonelli.it</t>
         </is>
       </c>
-      <c r="I80" t="n">
-        <v>44.6472046</v>
-      </c>
-      <c r="J80" t="n">
-        <v>10.9299876</v>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>44.6472046</t>
+        </is>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>10.9299876</t>
+        </is>
       </c>
     </row>
     <row r="81">
@@ -4294,11 +4610,15 @@
           <t>www.conservatoriopalermo.it</t>
         </is>
       </c>
-      <c r="I81" t="n">
-        <v>38.1213238</v>
-      </c>
-      <c r="J81" t="n">
-        <v>13.3640091</v>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>38.1213238</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>13.3640091</t>
+        </is>
       </c>
     </row>
     <row r="82">
@@ -4342,11 +4662,15 @@
           <t>www.conservatorio.pr.it</t>
         </is>
       </c>
-      <c r="I82" t="n">
-        <v>44.6952006</v>
-      </c>
-      <c r="J82" t="n">
-        <v>10.0979869</v>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>44.6952006</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>10.0979869</t>
+        </is>
       </c>
     </row>
     <row r="83">
@@ -4390,11 +4714,15 @@
           <t>www.conspv.it</t>
         </is>
       </c>
-      <c r="I83" t="n">
-        <v>45.1863517</v>
-      </c>
-      <c r="J83" t="n">
-        <v>9.162143199999999</v>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>45.1863517</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>9.1621432</t>
+        </is>
       </c>
     </row>
     <row r="84">
@@ -4438,11 +4766,15 @@
           <t>www.conservatorioperugia.it</t>
         </is>
       </c>
-      <c r="I84" t="n">
-        <v>43.1089834</v>
-      </c>
-      <c r="J84" t="n">
-        <v>12.3850994</v>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>43.1089834</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>12.3850994</t>
+        </is>
       </c>
     </row>
     <row r="85">
@@ -4486,11 +4818,15 @@
           <t>www.verdiravenna.it/</t>
         </is>
       </c>
-      <c r="I85" t="n">
-        <v>44.415086</v>
-      </c>
-      <c r="J85" t="n">
-        <v>12.2051541</v>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>44.4150860</t>
+        </is>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>12.2051541</t>
+        </is>
       </c>
     </row>
     <row r="86">
@@ -4534,11 +4870,15 @@
           <t>www.briccialditerni.it</t>
         </is>
       </c>
-      <c r="I86" t="n">
-        <v>42.5634291</v>
-      </c>
-      <c r="J86" t="n">
-        <v>12.6489197</v>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>42.5634291</t>
+        </is>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>12.6489197</t>
+        </is>
       </c>
     </row>
     <row r="87">
@@ -4582,11 +4922,15 @@
           <t>www.conservatoriotorino.eu</t>
         </is>
       </c>
-      <c r="I87" t="n">
-        <v>45.0629116</v>
-      </c>
-      <c r="J87" t="n">
-        <v>7.6847292</v>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>45.0629116</t>
+        </is>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>7.6847292</t>
+        </is>
       </c>
     </row>
     <row r="88">
@@ -4630,11 +4974,15 @@
           <t>www.conservatorio.tn.it/</t>
         </is>
       </c>
-      <c r="I88" t="n">
-        <v>45.8888242</v>
-      </c>
-      <c r="J88" t="n">
-        <v>10.8429772</v>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>45.8888242</t>
+        </is>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>10.8429772</t>
+        </is>
       </c>
     </row>
     <row r="89">
@@ -4678,11 +5026,15 @@
           <t>www.conservatorioverona.it</t>
         </is>
       </c>
-      <c r="I89" t="n">
-        <v>45.4452569</v>
-      </c>
-      <c r="J89" t="n">
-        <v>10.9989845</v>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>45.4452569</t>
+        </is>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>10.9989845</t>
+        </is>
       </c>
     </row>
     <row r="90">
@@ -4722,11 +5074,15 @@
         </is>
       </c>
       <c r="H90" t="inlineStr"/>
-      <c r="I90" t="n">
-        <v>45.0591181</v>
-      </c>
-      <c r="J90" t="n">
-        <v>12.0547219</v>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>45.0591181</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>12.0547219</t>
+        </is>
       </c>
     </row>
     <row r="91">
@@ -4770,11 +5126,15 @@
           <t>www.conservatoriovivaldi.it/</t>
         </is>
       </c>
-      <c r="I91" t="n">
-        <v>44.9124642</v>
-      </c>
-      <c r="J91" t="n">
-        <v>8.617315700000001</v>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>44.9124642</t>
+        </is>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>8.6173157</t>
+        </is>
       </c>
     </row>
     <row r="92">
@@ -4818,11 +5178,15 @@
           <t>www.conservatoriocimarosa.org</t>
         </is>
       </c>
-      <c r="I92" t="n">
-        <v>40.9161793</v>
-      </c>
-      <c r="J92" t="n">
-        <v>14.8012267</v>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>40.9161793</t>
+        </is>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>14.8012267</t>
+        </is>
       </c>
     </row>
     <row r="93">
@@ -4862,11 +5226,15 @@
         </is>
       </c>
       <c r="H93" t="inlineStr"/>
-      <c r="I93" t="n">
-        <v>41.1157586</v>
-      </c>
-      <c r="J93" t="n">
-        <v>16.8568829</v>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>41.1157586</t>
+        </is>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>16.8568829</t>
+        </is>
       </c>
     </row>
     <row r="94">
@@ -4910,11 +5278,15 @@
           <t>www.conservatorio.bn.it</t>
         </is>
       </c>
-      <c r="I94" t="n">
-        <v>41.130383</v>
-      </c>
-      <c r="J94" t="n">
-        <v>14.7821165</v>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>41.1303830</t>
+        </is>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>14.7821165</t>
+        </is>
       </c>
     </row>
     <row r="95">
@@ -4958,11 +5330,15 @@
           <t>www.consbo.it</t>
         </is>
       </c>
-      <c r="I95" t="n">
-        <v>44.4952952</v>
-      </c>
-      <c r="J95" t="n">
-        <v>11.3490593</v>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>44.4952952</t>
+        </is>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>11.3490593</t>
+        </is>
       </c>
     </row>
     <row r="96">
@@ -5006,11 +5382,15 @@
           <t>www.cons.bz.it</t>
         </is>
       </c>
-      <c r="I96" t="n">
-        <v>46.4976732</v>
-      </c>
-      <c r="J96" t="n">
-        <v>11.3515688</v>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>46.4976732</t>
+        </is>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>11.3515688</t>
+        </is>
       </c>
     </row>
     <row r="97">
@@ -5054,11 +5434,15 @@
           <t>www.consbs.it</t>
         </is>
       </c>
-      <c r="I97" t="n">
-        <v>45.5358028</v>
-      </c>
-      <c r="J97" t="n">
-        <v>10.2255838</v>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>45.5358028</t>
+        </is>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>10.2255838</t>
+        </is>
       </c>
     </row>
     <row r="98">
@@ -5102,11 +5486,15 @@
           <t>www.conservatoriocagliari.it</t>
         </is>
       </c>
-      <c r="I98" t="n">
-        <v>39.2171994</v>
-      </c>
-      <c r="J98" t="n">
-        <v>9.113310999999999</v>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>39.2171994</t>
+        </is>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>9.1133110</t>
+        </is>
       </c>
     </row>
     <row r="99">
@@ -5150,11 +5538,15 @@
           <t>www.Issmbellini.cl.it</t>
         </is>
       </c>
-      <c r="I99" t="n">
-        <v>37.4882462</v>
-      </c>
-      <c r="J99" t="n">
-        <v>14.0628911</v>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>37.4882462</t>
+        </is>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>14.0628911</t>
+        </is>
       </c>
     </row>
     <row r="100">
@@ -5198,11 +5590,15 @@
           <t>www.conservatorioperosi.it</t>
         </is>
       </c>
-      <c r="I100" t="n">
-        <v>41.7113278</v>
-      </c>
-      <c r="J100" t="n">
-        <v>14.9883469</v>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>41.7113278</t>
+        </is>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>14.9883469</t>
+        </is>
       </c>
     </row>
     <row r="101">
@@ -5246,11 +5642,15 @@
           <t>WWW.CONSCFV.IT</t>
         </is>
       </c>
-      <c r="I101" t="n">
-        <v>45.6721161</v>
-      </c>
-      <c r="J101" t="n">
-        <v>11.9248433</v>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>45.6721161</t>
+        </is>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>11.9248433</t>
+        </is>
       </c>
     </row>
     <row r="102">
@@ -5294,11 +5694,15 @@
           <t>www.conservatoriocatania.it</t>
         </is>
       </c>
-      <c r="I102" t="n">
-        <v>37.5203524</v>
-      </c>
-      <c r="J102" t="n">
-        <v>15.0822223</v>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>37.5203524</t>
+        </is>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>15.0822223</t>
+        </is>
       </c>
     </row>
     <row r="103">
@@ -5342,11 +5746,15 @@
           <t>www.madernalettimi.it</t>
         </is>
       </c>
-      <c r="I103" t="n">
-        <v>44.1373292</v>
-      </c>
-      <c r="J103" t="n">
-        <v>12.2531247</v>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>44.1373292</t>
+        </is>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>12.2531247</t>
+        </is>
       </c>
     </row>
     <row r="104">
@@ -5386,11 +5794,15 @@
         </is>
       </c>
       <c r="H104" t="inlineStr"/>
-      <c r="I104" t="n">
-        <v>45.8036294</v>
-      </c>
-      <c r="J104" t="n">
-        <v>9.0853398</v>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>45.8036294</t>
+        </is>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>9.0853398</t>
+        </is>
       </c>
     </row>
     <row r="105">
@@ -5434,11 +5846,15 @@
           <t>www.conservatoriocosenza.it</t>
         </is>
       </c>
-      <c r="I105" t="n">
-        <v>39.2840282</v>
-      </c>
-      <c r="J105" t="n">
-        <v>16.2587924</v>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>39.2840282</t>
+        </is>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>16.2587924</t>
+        </is>
       </c>
     </row>
     <row r="106">
@@ -5482,11 +5898,15 @@
           <t>www.conscremona.it/</t>
         </is>
       </c>
-      <c r="I106" t="n">
-        <v>45.1311839</v>
-      </c>
-      <c r="J106" t="n">
-        <v>10.0273548</v>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>45.1311839</t>
+        </is>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>10.0273548</t>
+        </is>
       </c>
     </row>
     <row r="107">
@@ -5526,11 +5946,15 @@
         </is>
       </c>
       <c r="H107" t="inlineStr"/>
-      <c r="I107" t="n">
-        <v>44.3931767</v>
-      </c>
-      <c r="J107" t="n">
-        <v>7.551703</v>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>44.3931767</t>
+        </is>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>7.5517030</t>
+        </is>
       </c>
     </row>
     <row r="108">
@@ -5570,11 +5994,15 @@
         </is>
       </c>
       <c r="H108" t="inlineStr"/>
-      <c r="I108" t="n">
-        <v>43.1617794</v>
-      </c>
-      <c r="J108" t="n">
-        <v>13.7173919</v>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>43.1617794</t>
+        </is>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>13.7173919</t>
+        </is>
       </c>
     </row>
     <row r="109">
@@ -5618,11 +6046,15 @@
           <t>www.conservatorioferrara.it</t>
         </is>
       </c>
-      <c r="I109" t="n">
-        <v>44.8382457</v>
-      </c>
-      <c r="J109" t="n">
-        <v>11.6220922</v>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>44.8382457</t>
+        </is>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>11.6220922</t>
+        </is>
       </c>
     </row>
     <row r="110">
@@ -5666,11 +6098,15 @@
           <t>www.consfi.it/</t>
         </is>
       </c>
-      <c r="I110" t="n">
-        <v>43.7763996</v>
-      </c>
-      <c r="J110" t="n">
-        <v>11.2583489</v>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>43.7763996</t>
+        </is>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>11.2583489</t>
+        </is>
       </c>
     </row>
     <row r="111">
@@ -5714,11 +6150,15 @@
           <t>www.conservatoriofoggia.it</t>
         </is>
       </c>
-      <c r="I111" t="n">
-        <v>41.5028106</v>
-      </c>
-      <c r="J111" t="n">
-        <v>15.4528939</v>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>41.5028106</t>
+        </is>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>15.4528939</t>
+        </is>
       </c>
     </row>
     <row r="112">
@@ -5762,11 +6202,15 @@
           <t>www.accademiabellearti.fr.it</t>
         </is>
       </c>
-      <c r="I112" t="n">
-        <v>41.5775271</v>
-      </c>
-      <c r="J112" t="n">
-        <v>13.6059872</v>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>41.5775271</t>
+        </is>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>13.6059872</t>
+        </is>
       </c>
     </row>
     <row r="113">
@@ -5810,11 +6254,15 @@
           <t>www.issmpuccinigallarate.it/</t>
         </is>
       </c>
-      <c r="I113" t="n">
-        <v>45.6650461</v>
-      </c>
-      <c r="J113" t="n">
-        <v>8.7884805</v>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>45.6650461</t>
+        </is>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>8.7884805</t>
+        </is>
       </c>
     </row>
     <row r="114">
@@ -5858,11 +6306,15 @@
           <t>www.accademialigustica.it/</t>
         </is>
       </c>
-      <c r="I114" t="n">
-        <v>44.4076284</v>
-      </c>
-      <c r="J114" t="n">
-        <v>8.9348449</v>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>44.4076284</t>
+        </is>
+      </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>8.9348449</t>
+        </is>
       </c>
     </row>
     <row r="115">
@@ -5902,11 +6354,15 @@
         </is>
       </c>
       <c r="H115" t="inlineStr"/>
-      <c r="I115" t="n">
-        <v>42.3552134</v>
-      </c>
-      <c r="J115" t="n">
-        <v>13.4151297</v>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>42.3552134</t>
+        </is>
+      </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>13.4151297</t>
+        </is>
       </c>
     </row>
     <row r="116">
@@ -5950,11 +6406,15 @@
           <t>www.conssp.it</t>
         </is>
       </c>
-      <c r="I116" t="n">
-        <v>44.1073249</v>
-      </c>
-      <c r="J116" t="n">
-        <v>9.826102000000001</v>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>44.1073249</t>
+        </is>
+      </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>9.8261020</t>
+        </is>
       </c>
     </row>
     <row r="117">
@@ -5998,11 +6458,15 @@
           <t>www.conslatina.it</t>
         </is>
       </c>
-      <c r="I117" t="n">
-        <v>41.4693594</v>
-      </c>
-      <c r="J117" t="n">
-        <v>12.9172571</v>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>41.4693594</t>
+        </is>
+      </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>12.9172571</t>
+        </is>
       </c>
     </row>
     <row r="118">
@@ -6042,11 +6506,15 @@
         </is>
       </c>
       <c r="H118" t="inlineStr"/>
-      <c r="I118" t="n">
-        <v>40.4373242</v>
-      </c>
-      <c r="J118" t="n">
-        <v>18.0273367</v>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>40.4373242</t>
+        </is>
+      </c>
+      <c r="J118" t="inlineStr">
+        <is>
+          <t>18.0273367</t>
+        </is>
       </c>
     </row>
     <row r="119">
@@ -6090,11 +6558,15 @@
           <t>www.consli.it</t>
         </is>
       </c>
-      <c r="I119" t="n">
-        <v>43.5560233</v>
-      </c>
-      <c r="J119" t="n">
-        <v>10.3173904</v>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>43.5560233</t>
+        </is>
+      </c>
+      <c r="J119" t="inlineStr">
+        <is>
+          <t>10.3173904</t>
+        </is>
       </c>
     </row>
     <row r="120">
@@ -6134,11 +6606,15 @@
         </is>
       </c>
       <c r="H120" t="inlineStr"/>
-      <c r="I120" t="n">
-        <v>43.8428292</v>
-      </c>
-      <c r="J120" t="n">
-        <v>10.5057569</v>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>43.8428292</t>
+        </is>
+      </c>
+      <c r="J120" t="inlineStr">
+        <is>
+          <t>10.5057569</t>
+        </is>
       </c>
     </row>
     <row r="121">
@@ -6182,11 +6658,15 @@
           <t>www.conservatoriomantova.com</t>
         </is>
       </c>
-      <c r="I121" t="n">
-        <v>45.1545324</v>
-      </c>
-      <c r="J121" t="n">
-        <v>10.7840711</v>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>45.1545324</t>
+        </is>
+      </c>
+      <c r="J121" t="inlineStr">
+        <is>
+          <t>10.7840711</t>
+        </is>
       </c>
     </row>
     <row r="122">
@@ -6230,11 +6710,15 @@
           <t>www.conservatoriomatera.it</t>
         </is>
       </c>
-      <c r="I122" t="n">
-        <v>40.6655731</v>
-      </c>
-      <c r="J122" t="n">
-        <v>16.609778</v>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>40.6655731</t>
+        </is>
+      </c>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t>16.6097780</t>
+        </is>
       </c>
     </row>
     <row r="123">
@@ -6278,11 +6762,15 @@
           <t>www.consme.it</t>
         </is>
       </c>
-      <c r="I123" t="n">
-        <v>38.1657684</v>
-      </c>
-      <c r="J123" t="n">
-        <v>15.5417453</v>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>38.1657684</t>
+        </is>
+      </c>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t>15.5417453</t>
+        </is>
       </c>
     </row>
     <row r="124">
@@ -6326,11 +6814,15 @@
           <t>www.consmi.it/</t>
         </is>
       </c>
-      <c r="I124" t="n">
-        <v>45.4650024</v>
-      </c>
-      <c r="J124" t="n">
-        <v>9.203199400000001</v>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>45.4650024</t>
+        </is>
+      </c>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t>9.2031994</t>
+        </is>
       </c>
     </row>
     <row r="125">
@@ -6370,11 +6862,15 @@
         </is>
       </c>
       <c r="H125" t="inlineStr"/>
-      <c r="I125" t="n">
-        <v>44.7835699</v>
-      </c>
-      <c r="J125" t="n">
-        <v>10.8854523</v>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>44.7835699</t>
+        </is>
+      </c>
+      <c r="J125" t="inlineStr">
+        <is>
+          <t>10.8854523</t>
+        </is>
       </c>
     </row>
     <row r="126">
@@ -6418,11 +6914,15 @@
           <t>www.conservatoriodimonopoli.org</t>
         </is>
       </c>
-      <c r="I126" t="n">
-        <v>40.9527986</v>
-      </c>
-      <c r="J126" t="n">
-        <v>17.2956015</v>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>40.9527986</t>
+        </is>
+      </c>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t>17.2956015</t>
+        </is>
       </c>
     </row>
     <row r="127">
@@ -6466,11 +6966,15 @@
           <t>www.sanpietroamajella.it</t>
         </is>
       </c>
-      <c r="I127" t="n">
-        <v>40.8358846</v>
-      </c>
-      <c r="J127" t="n">
-        <v>14.2487679</v>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>40.8358846</t>
+        </is>
+      </c>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t>14.2487679</t>
+        </is>
       </c>
     </row>
     <row r="128">
@@ -6514,11 +7018,15 @@
           <t>www.conscz.it</t>
         </is>
       </c>
-      <c r="I128" t="n">
-        <v>39.0368928</v>
-      </c>
-      <c r="J128" t="n">
-        <v>16.1607183</v>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>39.0368928</t>
+        </is>
+      </c>
+      <c r="J128" t="inlineStr">
+        <is>
+          <t>16.1607183</t>
+        </is>
       </c>
     </row>
     <row r="129">
@@ -6562,11 +7070,15 @@
           <t>www.consno.it</t>
         </is>
       </c>
-      <c r="I129" t="n">
-        <v>45.4444798</v>
-      </c>
-      <c r="J129" t="n">
-        <v>8.6202478</v>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>45.4444798</t>
+        </is>
+      </c>
+      <c r="J129" t="inlineStr">
+        <is>
+          <t>8.6202478</t>
+        </is>
       </c>
     </row>
     <row r="130">
@@ -6610,11 +7122,15 @@
           <t>www.conservatoriopollini.it/</t>
         </is>
       </c>
-      <c r="I130" t="n">
-        <v>45.4091816</v>
-      </c>
-      <c r="J130" t="n">
-        <v>11.8789892</v>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>45.4091816</t>
+        </is>
+      </c>
+      <c r="J130" t="inlineStr">
+        <is>
+          <t>11.8789892</t>
+        </is>
       </c>
     </row>
     <row r="131">
@@ -6658,11 +7174,15 @@
           <t>www.conservatoriopalermo.it/</t>
         </is>
       </c>
-      <c r="I131" t="n">
-        <v>38.1163595</v>
-      </c>
-      <c r="J131" t="n">
-        <v>13.3522738</v>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>38.1163595</t>
+        </is>
+      </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>13.3522738</t>
+        </is>
       </c>
     </row>
     <row r="132">
@@ -6702,11 +7222,15 @@
         </is>
       </c>
       <c r="H132" t="inlineStr"/>
-      <c r="I132" t="n">
-        <v>44.7997093</v>
-      </c>
-      <c r="J132" t="n">
-        <v>10.3247558</v>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>44.7997093</t>
+        </is>
+      </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>10.3247558</t>
+        </is>
       </c>
     </row>
     <row r="133">
@@ -6746,11 +7270,15 @@
         </is>
       </c>
       <c r="H133" t="inlineStr"/>
-      <c r="I133" t="n">
-        <v>45.1863517</v>
-      </c>
-      <c r="J133" t="n">
-        <v>9.162143199999999</v>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>45.1863517</t>
+        </is>
+      </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t>9.1621432</t>
+        </is>
       </c>
     </row>
     <row r="134">
@@ -6794,11 +7322,15 @@
           <t>www.abaperugia.org</t>
         </is>
       </c>
-      <c r="I134" t="n">
-        <v>43.1130349</v>
-      </c>
-      <c r="J134" t="n">
-        <v>12.38441</v>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>43.1130349</t>
+        </is>
+      </c>
+      <c r="J134" t="inlineStr">
+        <is>
+          <t>12.3844100</t>
+        </is>
       </c>
     </row>
     <row r="135">
@@ -6842,11 +7374,15 @@
           <t>www.conservatoriorossini.it</t>
         </is>
       </c>
-      <c r="I135" t="n">
-        <v>43.90921</v>
-      </c>
-      <c r="J135" t="n">
-        <v>12.9104169</v>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>43.9092100</t>
+        </is>
+      </c>
+      <c r="J135" t="inlineStr">
+        <is>
+          <t>12.9104169</t>
+        </is>
       </c>
     </row>
     <row r="136">
@@ -6890,11 +7426,15 @@
           <t>www.conservatoriope.it</t>
         </is>
       </c>
-      <c r="I136" t="n">
-        <v>42.4754123</v>
-      </c>
-      <c r="J136" t="n">
-        <v>14.2011306</v>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>42.4754123</t>
+        </is>
+      </c>
+      <c r="J136" t="inlineStr">
+        <is>
+          <t>14.2011306</t>
+        </is>
       </c>
     </row>
     <row r="137">
@@ -6938,11 +7478,15 @@
           <t>www.conservatorionicolini.com</t>
         </is>
       </c>
-      <c r="I137" t="n">
-        <v>45.0490767</v>
-      </c>
-      <c r="J137" t="n">
-        <v>9.6910176</v>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>45.0490767</t>
+        </is>
+      </c>
+      <c r="J137" t="inlineStr">
+        <is>
+          <t>9.6910176</t>
+        </is>
       </c>
     </row>
     <row r="138">
@@ -6986,11 +7530,15 @@
           <t>www.conservatoriopotenza.it</t>
         </is>
       </c>
-      <c r="I138" t="n">
-        <v>40.6392267</v>
-      </c>
-      <c r="J138" t="n">
-        <v>15.792239</v>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>40.6392267</t>
+        </is>
+      </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>15.7922390</t>
+        </is>
       </c>
     </row>
     <row r="139">
@@ -7034,11 +7582,15 @@
           <t>www.abaravenna.it</t>
         </is>
       </c>
-      <c r="I139" t="n">
-        <v>44.4262085</v>
-      </c>
-      <c r="J139" t="n">
-        <v>12.2137298</v>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>44.4262085</t>
+        </is>
+      </c>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>12.2137298</t>
+        </is>
       </c>
     </row>
     <row r="140">
@@ -7082,11 +7634,15 @@
           <t>www.conservatoriocilea.it</t>
         </is>
       </c>
-      <c r="I140" t="n">
-        <v>38.1178928</v>
-      </c>
-      <c r="J140" t="n">
-        <v>15.6578576</v>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>38.1178928</t>
+        </is>
+      </c>
+      <c r="J140" t="inlineStr">
+        <is>
+          <t>15.6578576</t>
+        </is>
       </c>
     </row>
     <row r="141">
@@ -7130,11 +7686,15 @@
           <t>www.peri-merulo.it/</t>
         </is>
       </c>
-      <c r="I141" t="n">
-        <v>44.6989596</v>
-      </c>
-      <c r="J141" t="n">
-        <v>10.6371242</v>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>44.6989596</t>
+        </is>
+      </c>
+      <c r="J141" t="inlineStr">
+        <is>
+          <t>10.6371242</t>
+        </is>
       </c>
     </row>
     <row r="142">
@@ -7178,11 +7738,15 @@
           <t>www.conservatoriotoscanini.it/</t>
         </is>
       </c>
-      <c r="I142" t="n">
-        <v>37.504695</v>
-      </c>
-      <c r="J142" t="n">
-        <v>13.2722009</v>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>37.5046950</t>
+        </is>
+      </c>
+      <c r="J142" t="inlineStr">
+        <is>
+          <t>13.2722009</t>
+        </is>
       </c>
     </row>
     <row r="143">
@@ -7226,11 +7790,15 @@
           <t>www.conservatoriosantacecilia.it</t>
         </is>
       </c>
-      <c r="I143" t="n">
-        <v>41.9074985</v>
-      </c>
-      <c r="J143" t="n">
-        <v>12.4788258</v>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>41.9074985</t>
+        </is>
+      </c>
+      <c r="J143" t="inlineStr">
+        <is>
+          <t>12.4788258</t>
+        </is>
       </c>
     </row>
     <row r="144">
@@ -7274,11 +7842,15 @@
           <t>www.conservatoriorovigo.it</t>
         </is>
       </c>
-      <c r="I144" t="n">
-        <v>45.0695569</v>
-      </c>
-      <c r="J144" t="n">
-        <v>11.7913368</v>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>45.0695569</t>
+        </is>
+      </c>
+      <c r="J144" t="inlineStr">
+        <is>
+          <t>11.7913368</t>
+        </is>
       </c>
     </row>
     <row r="145">
@@ -7322,11 +7894,15 @@
           <t>www.consalerno.it</t>
         </is>
       </c>
-      <c r="I145" t="n">
-        <v>40.6822539</v>
-      </c>
-      <c r="J145" t="n">
-        <v>14.7509898</v>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>40.6822539</t>
+        </is>
+      </c>
+      <c r="J145" t="inlineStr">
+        <is>
+          <t>14.7509898</t>
+        </is>
       </c>
     </row>
     <row r="146">
@@ -7370,11 +7946,15 @@
           <t>www.conservatorio.sassari.it/</t>
         </is>
       </c>
-      <c r="I146" t="n">
-        <v>40.7234746</v>
-      </c>
-      <c r="J146" t="n">
-        <v>8.5612674</v>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>40.7234746</t>
+        </is>
+      </c>
+      <c r="J146" t="inlineStr">
+        <is>
+          <t>8.5612674</t>
+        </is>
       </c>
     </row>
     <row r="147">
@@ -7418,11 +7998,15 @@
           <t>www.conservatoriosiena.it/it</t>
         </is>
       </c>
-      <c r="I147" t="n">
-        <v>43.3145921</v>
-      </c>
-      <c r="J147" t="n">
-        <v>11.3307638</v>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>43.3145921</t>
+        </is>
+      </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>11.3307638</t>
+        </is>
       </c>
     </row>
     <row r="148">
@@ -7466,11 +8050,15 @@
           <t>www.paisiello.it</t>
         </is>
       </c>
-      <c r="I148" t="n">
-        <v>40.4749097</v>
-      </c>
-      <c r="J148" t="n">
-        <v>17.2312876</v>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>40.4749097</t>
+        </is>
+      </c>
+      <c r="J148" t="inlineStr">
+        <is>
+          <t>17.2312876</t>
+        </is>
       </c>
     </row>
     <row r="149">
@@ -7514,11 +8102,15 @@
           <t>www.conservatoriobraga.it</t>
         </is>
       </c>
-      <c r="I149" t="n">
-        <v>42.6601486</v>
-      </c>
-      <c r="J149" t="n">
-        <v>13.7007032</v>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>42.6601486</t>
+        </is>
+      </c>
+      <c r="J149" t="inlineStr">
+        <is>
+          <t>13.7007032</t>
+        </is>
       </c>
     </row>
     <row r="150">
@@ -7558,11 +8150,15 @@
         </is>
       </c>
       <c r="H150" t="inlineStr"/>
-      <c r="I150" t="n">
-        <v>42.6539486</v>
-      </c>
-      <c r="J150" t="n">
-        <v>12.4396528</v>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>42.6539486</t>
+        </is>
+      </c>
+      <c r="J150" t="inlineStr">
+        <is>
+          <t>12.4396528</t>
+        </is>
       </c>
     </row>
     <row r="151">
@@ -7606,11 +8202,15 @@
           <t>www.albertina.academy</t>
         </is>
       </c>
-      <c r="I151" t="n">
-        <v>45.0675807</v>
-      </c>
-      <c r="J151" t="n">
-        <v>7.6897297</v>
+      <c r="I151" t="inlineStr">
+        <is>
+          <t>45.0675807</t>
+        </is>
+      </c>
+      <c r="J151" t="inlineStr">
+        <is>
+          <t>7.6897297</t>
+        </is>
       </c>
     </row>
     <row r="152">
@@ -7654,11 +8254,15 @@
           <t>www.constp.it</t>
         </is>
       </c>
-      <c r="I152" t="n">
-        <v>38.0123644</v>
-      </c>
-      <c r="J152" t="n">
-        <v>12.5649772</v>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>38.0123644</t>
+        </is>
+      </c>
+      <c r="J152" t="inlineStr">
+        <is>
+          <t>12.5649772</t>
+        </is>
       </c>
     </row>
     <row r="153">
@@ -7702,11 +8306,15 @@
           <t>www.conservatorio.tn.it/</t>
         </is>
       </c>
-      <c r="I153" t="n">
-        <v>46.0685654</v>
-      </c>
-      <c r="J153" t="n">
-        <v>11.1255906</v>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>46.0685654</t>
+        </is>
+      </c>
+      <c r="J153" t="inlineStr">
+        <is>
+          <t>11.1255906</t>
+        </is>
       </c>
     </row>
     <row r="154">
@@ -7750,11 +8358,15 @@
           <t>www.conts.it</t>
         </is>
       </c>
-      <c r="I154" t="n">
-        <v>45.6558027</v>
-      </c>
-      <c r="J154" t="n">
-        <v>13.7750136</v>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>45.6558027</t>
+        </is>
+      </c>
+      <c r="J154" t="inlineStr">
+        <is>
+          <t>13.7750136</t>
+        </is>
       </c>
     </row>
     <row r="155">
@@ -7794,11 +8406,15 @@
         </is>
       </c>
       <c r="H155" t="inlineStr"/>
-      <c r="I155" t="n">
-        <v>46.0651811</v>
-      </c>
-      <c r="J155" t="n">
-        <v>13.2397028</v>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>46.0651811</t>
+        </is>
+      </c>
+      <c r="J155" t="inlineStr">
+        <is>
+          <t>13.2397028</t>
+        </is>
       </c>
     </row>
     <row r="156">
@@ -7842,11 +8458,15 @@
           <t>www.conservatoriovenezia.eu</t>
         </is>
       </c>
-      <c r="I156" t="n">
-        <v>45.4323575</v>
-      </c>
-      <c r="J156" t="n">
-        <v>12.3304966</v>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>45.4323575</t>
+        </is>
+      </c>
+      <c r="J156" t="inlineStr">
+        <is>
+          <t>12.3304966</t>
+        </is>
       </c>
     </row>
     <row r="157">
@@ -7890,11 +8510,15 @@
           <t>www.accademiabelleartiverona.it/it/</t>
         </is>
       </c>
-      <c r="I157" t="n">
-        <v>45.4989147</v>
-      </c>
-      <c r="J157" t="n">
-        <v>10.9390044</v>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>45.4989147</t>
+        </is>
+      </c>
+      <c r="J157" t="inlineStr">
+        <is>
+          <t>10.9390044</t>
+        </is>
       </c>
     </row>
     <row r="158">
@@ -7938,11 +8562,15 @@
           <t>www.consvv.it</t>
         </is>
       </c>
-      <c r="I158" t="n">
-        <v>38.6261714</v>
-      </c>
-      <c r="J158" t="n">
-        <v>15.8630754</v>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>38.6261714</t>
+        </is>
+      </c>
+      <c r="J158" t="inlineStr">
+        <is>
+          <t>15.8630754</t>
+        </is>
       </c>
     </row>
     <row r="159">
@@ -7986,11 +8614,15 @@
           <t>www.consvi.it/</t>
         </is>
       </c>
-      <c r="I159" t="n">
-        <v>45.550678</v>
-      </c>
-      <c r="J159" t="n">
-        <v>11.554186</v>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>45.5506780</t>
+        </is>
+      </c>
+      <c r="J159" t="inlineStr">
+        <is>
+          <t>11.5541860</t>
+        </is>
       </c>
     </row>
     <row r="160">
@@ -8034,11 +8666,15 @@
           <t>www.cpm.it</t>
         </is>
       </c>
-      <c r="I160" t="n">
-        <v>45.507534</v>
-      </c>
-      <c r="J160" t="n">
-        <v>9.2033463</v>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>45.5075340</t>
+        </is>
+      </c>
+      <c r="J160" t="inlineStr">
+        <is>
+          <t>9.2033463</t>
+        </is>
       </c>
     </row>
     <row r="161">
@@ -8082,11 +8718,15 @@
           <t>www.isiafaenza.it</t>
         </is>
       </c>
-      <c r="I161" t="n">
-        <v>44.2870556</v>
-      </c>
-      <c r="J161" t="n">
-        <v>11.8801787</v>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>44.2870556</t>
+        </is>
+      </c>
+      <c r="J161" t="inlineStr">
+        <is>
+          <t>11.8801787</t>
+        </is>
       </c>
     </row>
     <row r="162">
@@ -8130,11 +8770,15 @@
           <t>www.isiadesign.fi.it/</t>
         </is>
       </c>
-      <c r="I162" t="n">
-        <v>43.7722975</v>
-      </c>
-      <c r="J162" t="n">
-        <v>11.2304322</v>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>43.7722975</t>
+        </is>
+      </c>
+      <c r="J162" t="inlineStr">
+        <is>
+          <t>11.2304322</t>
+        </is>
       </c>
     </row>
     <row r="163">
@@ -8178,11 +8822,15 @@
           <t>www.isiadesign.pe.it</t>
         </is>
       </c>
-      <c r="I163" t="n">
-        <v>42.4745581</v>
-      </c>
-      <c r="J163" t="n">
-        <v>14.2035856</v>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>42.4745581</t>
+        </is>
+      </c>
+      <c r="J163" t="inlineStr">
+        <is>
+          <t>14.2035856</t>
+        </is>
       </c>
     </row>
     <row r="164">
@@ -8226,11 +8874,15 @@
           <t>www.isiaroma.it</t>
         </is>
       </c>
-      <c r="I164" t="n">
-        <v>41.9001808</v>
-      </c>
-      <c r="J164" t="n">
-        <v>12.4766899</v>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>41.9001808</t>
+        </is>
+      </c>
+      <c r="J164" t="inlineStr">
+        <is>
+          <t>12.4766899</t>
+        </is>
       </c>
     </row>
     <row r="165">
@@ -8274,11 +8926,15 @@
           <t>www.isiaurbino.net</t>
         </is>
       </c>
-      <c r="I165" t="n">
-        <v>43.7232891</v>
-      </c>
-      <c r="J165" t="n">
-        <v>12.6375713</v>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>43.7232891</t>
+        </is>
+      </c>
+      <c r="J165" t="inlineStr">
+        <is>
+          <t>12.6375713</t>
+        </is>
       </c>
     </row>
     <row r="166">
@@ -8289,7 +8945,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -8322,11 +8978,15 @@
           <t>www.iaad.it</t>
         </is>
       </c>
-      <c r="I166" t="n">
-        <v>45.0679702</v>
-      </c>
-      <c r="J166" t="n">
-        <v>7.6820983</v>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>45.0679702</t>
+        </is>
+      </c>
+      <c r="J166" t="inlineStr">
+        <is>
+          <t>7.6820983</t>
+        </is>
       </c>
     </row>
     <row r="167">
@@ -8337,7 +8997,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -8370,11 +9030,15 @@
           <t>www.istitutodeldesign.it</t>
         </is>
       </c>
-      <c r="I167" t="n">
-        <v>40.6601928</v>
-      </c>
-      <c r="J167" t="n">
-        <v>16.606458</v>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>40.6601928</t>
+        </is>
+      </c>
+      <c r="J167" t="inlineStr">
+        <is>
+          <t>16.6064580</t>
+        </is>
       </c>
     </row>
     <row r="168">
@@ -8385,7 +9049,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -8414,11 +9078,15 @@
           <t>www.ied.it</t>
         </is>
       </c>
-      <c r="I168" t="n">
-        <v>39.2171994</v>
-      </c>
-      <c r="J168" t="n">
-        <v>9.113310999999999</v>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>39.2171994</t>
+        </is>
+      </c>
+      <c r="J168" t="inlineStr">
+        <is>
+          <t>9.1133110</t>
+        </is>
       </c>
     </row>
     <row r="169">
@@ -8429,7 +9097,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -8458,11 +9126,15 @@
           <t>www.ied.it</t>
         </is>
       </c>
-      <c r="I169" t="n">
-        <v>43.7697955</v>
-      </c>
-      <c r="J169" t="n">
-        <v>11.2556404</v>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>43.7697955</t>
+        </is>
+      </c>
+      <c r="J169" t="inlineStr">
+        <is>
+          <t>11.2556404</t>
+        </is>
       </c>
     </row>
     <row r="170">
@@ -8473,7 +9145,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -8502,11 +9174,15 @@
           <t>www.ied.it</t>
         </is>
       </c>
-      <c r="I170" t="n">
-        <v>45.4641943</v>
-      </c>
-      <c r="J170" t="n">
-        <v>9.1896346</v>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>45.4641943</t>
+        </is>
+      </c>
+      <c r="J170" t="inlineStr">
+        <is>
+          <t>9.1896346</t>
+        </is>
       </c>
     </row>
     <row r="171">
@@ -8517,7 +9193,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -8546,11 +9222,15 @@
           <t>www.ied.it</t>
         </is>
       </c>
-      <c r="I171" t="n">
-        <v>41.8933203</v>
-      </c>
-      <c r="J171" t="n">
-        <v>12.4829321</v>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>41.8933203</t>
+        </is>
+      </c>
+      <c r="J171" t="inlineStr">
+        <is>
+          <t>12.4829321</t>
+        </is>
       </c>
     </row>
     <row r="172">
@@ -8561,7 +9241,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -8590,11 +9270,15 @@
           <t>www.ied.it</t>
         </is>
       </c>
-      <c r="I172" t="n">
-        <v>45.0677551</v>
-      </c>
-      <c r="J172" t="n">
-        <v>7.6824892</v>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>45.0677551</t>
+        </is>
+      </c>
+      <c r="J172" t="inlineStr">
+        <is>
+          <t>7.6824892</t>
+        </is>
       </c>
     </row>
     <row r="173">
@@ -8605,7 +9289,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -8638,11 +9322,15 @@
           <t>www.istitutoitalianodesign.it/</t>
         </is>
       </c>
-      <c r="I173" t="n">
-        <v>43.1121562</v>
-      </c>
-      <c r="J173" t="n">
-        <v>12.3907473</v>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>43.1121562</t>
+        </is>
+      </c>
+      <c r="J173" t="inlineStr">
+        <is>
+          <t>12.3907473</t>
+        </is>
       </c>
     </row>
     <row r="174">
@@ -8653,7 +9341,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -8686,11 +9374,15 @@
           <t>www.istitutomarangoni.com</t>
         </is>
       </c>
-      <c r="I174" t="n">
-        <v>45.4276613</v>
-      </c>
-      <c r="J174" t="n">
-        <v>9.0495351</v>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>45.4276613</t>
+        </is>
+      </c>
+      <c r="J174" t="inlineStr">
+        <is>
+          <t>9.0495351</t>
+        </is>
       </c>
     </row>
     <row r="175">
@@ -8701,7 +9393,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -8734,11 +9426,15 @@
           <t>www.istitutomarangoni.com</t>
         </is>
       </c>
-      <c r="I175" t="n">
-        <v>43.7697955</v>
-      </c>
-      <c r="J175" t="n">
-        <v>11.2556404</v>
+      <c r="I175" t="inlineStr">
+        <is>
+          <t>43.7697955</t>
+        </is>
+      </c>
+      <c r="J175" t="inlineStr">
+        <is>
+          <t>11.2556404</t>
+        </is>
       </c>
     </row>
     <row r="176">
@@ -8749,7 +9445,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -8782,11 +9478,15 @@
           <t>www.modartech.com</t>
         </is>
       </c>
-      <c r="I176" t="n">
-        <v>43.6614004</v>
-      </c>
-      <c r="J176" t="n">
-        <v>10.6295127</v>
+      <c r="I176" t="inlineStr">
+        <is>
+          <t>43.6614004</t>
+        </is>
+      </c>
+      <c r="J176" t="inlineStr">
+        <is>
+          <t>10.6295127</t>
+        </is>
       </c>
     </row>
     <row r="177">
@@ -8797,7 +9497,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -8830,11 +9530,15 @@
           <t>www.istitutopantheon.com</t>
         </is>
       </c>
-      <c r="I177" t="n">
-        <v>41.8997872</v>
-      </c>
-      <c r="J177" t="n">
-        <v>12.4768054</v>
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>41.8997872</t>
+        </is>
+      </c>
+      <c r="J177" t="inlineStr">
+        <is>
+          <t>12.4768054</t>
+        </is>
       </c>
     </row>
     <row r="178">
@@ -8845,7 +9549,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -8878,11 +9582,15 @@
           <t>www.galileovd.it</t>
         </is>
       </c>
-      <c r="I178" t="n">
-        <v>45.3951622</v>
-      </c>
-      <c r="J178" t="n">
-        <v>11.9302126</v>
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>45.3951622</t>
+        </is>
+      </c>
+      <c r="J178" t="inlineStr">
+        <is>
+          <t>11.9302126</t>
+        </is>
       </c>
     </row>
     <row r="179">
@@ -8893,7 +9601,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Altro</t>
+          <t>Accademie di Belle Arti</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -8926,11 +9634,15 @@
           <t>www.poliarte.net</t>
         </is>
       </c>
-      <c r="I179" t="n">
-        <v>43.6066245</v>
-      </c>
-      <c r="J179" t="n">
-        <v>13.5099099</v>
+      <c r="I179" t="inlineStr">
+        <is>
+          <t>43.6066245</t>
+        </is>
+      </c>
+      <c r="J179" t="inlineStr">
+        <is>
+          <t>13.5099099</t>
+        </is>
       </c>
     </row>
     <row r="180">
@@ -8941,7 +9653,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -8974,11 +9686,15 @@
           <t>www.quasarinstitute.it</t>
         </is>
       </c>
-      <c r="I180" t="n">
-        <v>41.9053413</v>
-      </c>
-      <c r="J180" t="n">
-        <v>12.4675403</v>
+      <c r="I180" t="inlineStr">
+        <is>
+          <t>41.9053413</t>
+        </is>
+      </c>
+      <c r="J180" t="inlineStr">
+        <is>
+          <t>12.4675403</t>
+        </is>
       </c>
     </row>
     <row r="181">
@@ -8989,7 +9705,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -9022,11 +9738,15 @@
           <t>www.secoli.com</t>
         </is>
       </c>
-      <c r="I181" t="n">
-        <v>45.5247729</v>
-      </c>
-      <c r="J181" t="n">
-        <v>9.368399399999999</v>
+      <c r="I181" t="inlineStr">
+        <is>
+          <t>45.5247729</t>
+        </is>
+      </c>
+      <c r="J181" t="inlineStr">
+        <is>
+          <t>9.3683994</t>
+        </is>
       </c>
     </row>
     <row r="182">
@@ -9070,11 +9790,15 @@
           <t>www.conservatoriobraga.it</t>
         </is>
       </c>
-      <c r="I182" t="n">
-        <v>42.658118</v>
-      </c>
-      <c r="J182" t="n">
-        <v>13.6978746</v>
+      <c r="I182" t="inlineStr">
+        <is>
+          <t>42.6581180</t>
+        </is>
+      </c>
+      <c r="J182" t="inlineStr">
+        <is>
+          <t>13.6978746</t>
+        </is>
       </c>
     </row>
     <row r="183">
@@ -9118,11 +9842,15 @@
           <t>www.isiaroma.it/</t>
         </is>
       </c>
-      <c r="I183" t="n">
-        <v>45.9562503</v>
-      </c>
-      <c r="J183" t="n">
-        <v>12.6597197</v>
+      <c r="I183" t="inlineStr">
+        <is>
+          <t>45.9562503</t>
+        </is>
+      </c>
+      <c r="J183" t="inlineStr">
+        <is>
+          <t>12.6597197</t>
+        </is>
       </c>
     </row>
     <row r="184">
@@ -9166,11 +9894,15 @@
           <t>www.laba.edu</t>
         </is>
       </c>
-      <c r="I184" t="n">
-        <v>45.5593936</v>
-      </c>
-      <c r="J184" t="n">
-        <v>10.2036264</v>
+      <c r="I184" t="inlineStr">
+        <is>
+          <t>45.5593936</t>
+        </is>
+      </c>
+      <c r="J184" t="inlineStr">
+        <is>
+          <t>10.2036264</t>
+        </is>
       </c>
     </row>
     <row r="185">
@@ -9214,11 +9946,15 @@
           <t>www.laba.biz</t>
         </is>
       </c>
-      <c r="I185" t="n">
-        <v>43.7556414</v>
-      </c>
-      <c r="J185" t="n">
-        <v>11.2985995</v>
+      <c r="I185" t="inlineStr">
+        <is>
+          <t>43.7556414</t>
+        </is>
+      </c>
+      <c r="J185" t="inlineStr">
+        <is>
+          <t>11.2985995</t>
+        </is>
       </c>
     </row>
     <row r="186">
@@ -9262,11 +9998,15 @@
           <t>www.accademia.rimini.it</t>
         </is>
       </c>
-      <c r="I186" t="n">
-        <v>44.0620718</v>
-      </c>
-      <c r="J186" t="n">
-        <v>12.574592</v>
+      <c r="I186" t="inlineStr">
+        <is>
+          <t>44.0620718</t>
+        </is>
+      </c>
+      <c r="J186" t="inlineStr">
+        <is>
+          <t>12.5745920</t>
+        </is>
       </c>
     </row>
     <row r="187">
@@ -9306,11 +10046,15 @@
         </is>
       </c>
       <c r="H187" t="inlineStr"/>
-      <c r="I187" t="n">
-        <v>45.4455443</v>
-      </c>
-      <c r="J187" t="n">
-        <v>9.1743922</v>
+      <c r="I187" t="inlineStr">
+        <is>
+          <t>45.4455443</t>
+        </is>
+      </c>
+      <c r="J187" t="inlineStr">
+        <is>
+          <t>9.1743922</t>
+        </is>
       </c>
     </row>
     <row r="188">
@@ -9354,11 +10098,15 @@
           <t>www.poliartibg.it/</t>
         </is>
       </c>
-      <c r="I188" t="n">
-        <v>45.6699405</v>
-      </c>
-      <c r="J188" t="n">
-        <v>9.6309699</v>
+      <c r="I188" t="inlineStr">
+        <is>
+          <t>45.6699405</t>
+        </is>
+      </c>
+      <c r="J188" t="inlineStr">
+        <is>
+          <t>9.6309699</t>
+        </is>
       </c>
     </row>
     <row r="189">
@@ -9402,11 +10150,15 @@
           <t>www.accademiacarrara.it</t>
         </is>
       </c>
-      <c r="I189" t="n">
-        <v>45.6601869</v>
-      </c>
-      <c r="J189" t="n">
-        <v>9.674451299999999</v>
+      <c r="I189" t="inlineStr">
+        <is>
+          <t>45.6601869</t>
+        </is>
+      </c>
+      <c r="J189" t="inlineStr">
+        <is>
+          <t>9.6744513</t>
+        </is>
       </c>
     </row>
     <row r="190">
@@ -9450,11 +10202,15 @@
           <t>www.consbg.it/</t>
         </is>
       </c>
-      <c r="I190" t="n">
-        <v>45.7033389</v>
-      </c>
-      <c r="J190" t="n">
-        <v>9.6608543</v>
+      <c r="I190" t="inlineStr">
+        <is>
+          <t>45.7033389</t>
+        </is>
+      </c>
+      <c r="J190" t="inlineStr">
+        <is>
+          <t>9.6608543</t>
+        </is>
       </c>
     </row>
     <row r="191">
@@ -9465,7 +10221,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
@@ -9498,11 +10254,15 @@
           <t>www.rafflesmilano.it</t>
         </is>
       </c>
-      <c r="I191" t="n">
-        <v>45.4784738</v>
-      </c>
-      <c r="J191" t="n">
-        <v>9.204465000000001</v>
+      <c r="I191" t="inlineStr">
+        <is>
+          <t>45.4784738</t>
+        </is>
+      </c>
+      <c r="J191" t="inlineStr">
+        <is>
+          <t>9.2044650</t>
+        </is>
       </c>
     </row>
     <row r="192">
@@ -9546,11 +10306,15 @@
           <t>www.rafflesmilano.it</t>
         </is>
       </c>
-      <c r="I192" t="n">
-        <v>45.4784738</v>
-      </c>
-      <c r="J192" t="n">
-        <v>9.204465000000001</v>
+      <c r="I192" t="inlineStr">
+        <is>
+          <t>45.4784738</t>
+        </is>
+      </c>
+      <c r="J192" t="inlineStr">
+        <is>
+          <t>9.2044650</t>
+        </is>
       </c>
     </row>
     <row r="193">
@@ -9594,11 +10358,15 @@
           <t>www.unirufa.it</t>
         </is>
       </c>
-      <c r="I193" t="n">
-        <v>41.9238813</v>
-      </c>
-      <c r="J193" t="n">
-        <v>12.5060905</v>
+      <c r="I193" t="inlineStr">
+        <is>
+          <t>41.9238813</t>
+        </is>
+      </c>
+      <c r="J193" t="inlineStr">
+        <is>
+          <t>12.5060905</t>
+        </is>
       </c>
     </row>
     <row r="194">
@@ -9642,11 +10410,15 @@
           <t>www.unirufa.it/sedi/campus-milano-scalo-farini/</t>
         </is>
       </c>
-      <c r="I194" t="n">
-        <v>45.4975743</v>
-      </c>
-      <c r="J194" t="n">
-        <v>9.1657063</v>
+      <c r="I194" t="inlineStr">
+        <is>
+          <t>45.4975743</t>
+        </is>
+      </c>
+      <c r="J194" t="inlineStr">
+        <is>
+          <t>9.1657063</t>
+        </is>
       </c>
     </row>
     <row r="195">
@@ -9657,7 +10429,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Istituti di Design, Moda e Belle Arti</t>
+          <t>Istituti di Design e Moda</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -9686,27 +10458,31 @@
         </is>
       </c>
       <c r="H195" t="inlineStr"/>
-      <c r="I195" t="n">
-        <v>45.4727782</v>
-      </c>
-      <c r="J195" t="n">
-        <v>9.2420901</v>
+      <c r="I195" t="inlineStr">
+        <is>
+          <t>45.4727782</t>
+        </is>
+      </c>
+      <c r="J195" t="inlineStr">
+        <is>
+          <t>9.2420901</t>
+        </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>saint-louis-college-of-music</t>
+          <t>saint-louis-music-center-college-of-music-di-milano</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Istituti Musicali</t>
+          <t>Altro</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>Saint Louis College of Music</t>
+          <t>Saint Louis Music Center - College Of Music di Milano</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
@@ -9719,34 +10495,46 @@
           <t>Decentrata</t>
         </is>
       </c>
-      <c r="F196" t="inlineStr"/>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>Viale L. Bodio, 37, 20158, Milano, Mi, Italia</t>
+        </is>
+      </c>
       <c r="G196" t="inlineStr">
         <is>
           <t>Privato</t>
         </is>
       </c>
-      <c r="H196" t="inlineStr"/>
-      <c r="I196" t="n">
-        <v>45.4641943</v>
-      </c>
-      <c r="J196" t="n">
-        <v>9.1896346</v>
+      <c r="H196" t="inlineStr">
+        <is>
+          <t>www.slmc.it</t>
+        </is>
+      </c>
+      <c r="I196" t="inlineStr">
+        <is>
+          <t>45.4641943</t>
+        </is>
+      </c>
+      <c r="J196" t="inlineStr">
+        <is>
+          <t>9.1896346</t>
+        </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>saint-louis-college-of-music</t>
+          <t>saint-louis-music-center-college-of-music-di-roma</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Istituti Musicali</t>
+          <t>Altro</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>Saint Louis College of Music</t>
+          <t>Saint Louis Music Center - College Of Music di Roma</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
@@ -9759,39 +10547,51 @@
           <t>Principale</t>
         </is>
       </c>
-      <c r="F197" t="inlineStr"/>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>Via Baccina, 47, 00184 Roma, RM, Italia</t>
+        </is>
+      </c>
       <c r="G197" t="inlineStr">
         <is>
           <t>Privato</t>
         </is>
       </c>
-      <c r="H197" t="inlineStr"/>
-      <c r="I197" t="n">
-        <v>41.8948917</v>
-      </c>
-      <c r="J197" t="n">
-        <v>12.4901637</v>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>www.slmc.it</t>
+        </is>
+      </c>
+      <c r="I197" t="inlineStr">
+        <is>
+          <t>41.8948917</t>
+        </is>
+      </c>
+      <c r="J197" t="inlineStr">
+        <is>
+          <t>12.4901637</t>
+        </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>saint-louis-music-center-college-of-music-di-roma</t>
+          <t>scuola-del-teatro-musicale-stm</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Altro</t>
+          <t>Istituti di Teatro e Coreutica</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>Saint Louis Music Center - College Of Music di Roma</t>
+          <t>Scuola del Teatro Musicale (STM)</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>Roma</t>
+          <t>Novara</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
@@ -9801,7 +10601,7 @@
       </c>
       <c r="F198" t="inlineStr">
         <is>
-          <t>Via Baccina, 47, 00184 Roma, RM, Italia</t>
+          <t>Piazza Martiri della Libertà 2 , 28100, Novara, No, , Italia</t>
         </is>
       </c>
       <c r="G198" t="inlineStr">
@@ -9811,35 +10611,39 @@
       </c>
       <c r="H198" t="inlineStr">
         <is>
-          <t>www.slmc.it</t>
-        </is>
-      </c>
-      <c r="I198" t="n">
-        <v>41.8948917</v>
-      </c>
-      <c r="J198" t="n">
-        <v>12.4901637</v>
+          <t>www.scuolateatromusicale.it</t>
+        </is>
+      </c>
+      <c r="I198" t="inlineStr">
+        <is>
+          <t>45.4452698</t>
+        </is>
+      </c>
+      <c r="J198" t="inlineStr">
+        <is>
+          <t>8.6180529</t>
+        </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>scuola-del-teatro-musicale-stm</t>
+          <t>scuola-di-musica-di-fiesole</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Istituti di Teatro e Coreutica</t>
+          <t>Istituti Musicali</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>Scuola del Teatro Musicale (STM)</t>
+          <t>Scuola di Musica di Fiesole</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>Novara</t>
+          <t>Fiesole</t>
         </is>
       </c>
       <c r="E199" t="inlineStr">
@@ -9849,7 +10653,7 @@
       </c>
       <c r="F199" t="inlineStr">
         <is>
-          <t>Piazza Martiri della Libertà 2 , 28100, Novara, No, , Italia</t>
+          <t>Piazza Mino da Fiesole, 32a, 50014, Fiesole, Fi, , Italia</t>
         </is>
       </c>
       <c r="G199" t="inlineStr">
@@ -9859,35 +10663,39 @@
       </c>
       <c r="H199" t="inlineStr">
         <is>
-          <t>www.scuolateatromusicale.it</t>
-        </is>
-      </c>
-      <c r="I199" t="n">
-        <v>45.4452698</v>
-      </c>
-      <c r="J199" t="n">
-        <v>8.6180529</v>
+          <t>www.scuolamusicafiesole.it</t>
+        </is>
+      </c>
+      <c r="I199" t="inlineStr">
+        <is>
+          <t>43.8064116</t>
+        </is>
+      </c>
+      <c r="J199" t="inlineStr">
+        <is>
+          <t>11.2929501</t>
+        </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>scuola-di-musica-di-fiesole</t>
+          <t>the-bernstein-school-of-musical-theater</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Istituti Musicali</t>
+          <t>Istituti di Teatro e Coreutica</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>Scuola di Musica di Fiesole</t>
+          <t>The Bernstein School of Musical Theater</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>Fiesole</t>
+          <t>Bologna</t>
         </is>
       </c>
       <c r="E200" t="inlineStr">
@@ -9897,7 +10705,7 @@
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>Piazza Mino da Fiesole, 32a, 50014, Fiesole, Fi, , Italia</t>
+          <t>Via Paolo Nanni Costa 12/6, 40133, Bologna, Bo, , Italia</t>
         </is>
       </c>
       <c r="G200" t="inlineStr">
@@ -9907,62 +10715,18 @@
       </c>
       <c r="H200" t="inlineStr">
         <is>
-          <t>www.scuolamusicafiesole.it</t>
-        </is>
-      </c>
-      <c r="I200" t="n">
-        <v>43.8064116</v>
-      </c>
-      <c r="J200" t="n">
-        <v>11.2929501</v>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" t="inlineStr">
-        <is>
-          <t>the-bernstein-school-of-musical-theater</t>
-        </is>
-      </c>
-      <c r="B201" t="inlineStr">
-        <is>
-          <t>Istituti di Teatro e Coreutica</t>
-        </is>
-      </c>
-      <c r="C201" t="inlineStr">
-        <is>
-          <t>The Bernstein School of Musical Theater</t>
-        </is>
-      </c>
-      <c r="D201" t="inlineStr">
-        <is>
-          <t>Bologna</t>
-        </is>
-      </c>
-      <c r="E201" t="inlineStr">
-        <is>
-          <t>Principale</t>
-        </is>
-      </c>
-      <c r="F201" t="inlineStr">
-        <is>
-          <t>Via Paolo Nanni Costa 12/6, 40133, Bologna, Bo, , Italia</t>
-        </is>
-      </c>
-      <c r="G201" t="inlineStr">
-        <is>
-          <t>Privato</t>
-        </is>
-      </c>
-      <c r="H201" t="inlineStr">
-        <is>
           <t>www.bsmt.it/</t>
         </is>
       </c>
-      <c r="I201" t="n">
-        <v>44.5073503</v>
-      </c>
-      <c r="J201" t="n">
-        <v>11.3066727</v>
+      <c r="I200" t="inlineStr">
+        <is>
+          <t>44.5073503</t>
+        </is>
+      </c>
+      <c r="J200" t="inlineStr">
+        <is>
+          <t>11.3066727</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>